<commit_message>
Replaced 2012-0 with 2012
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RES_DemandFractions.xlsx
+++ b/SuppXLS/Scen_RES_DemandFractions.xlsx
@@ -112,8 +112,8 @@
     <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0;\-\ #,##0;_-\ &quot;- &quot;"/>
     <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="34" x14ac:knownFonts="1">
     <font>
@@ -915,7 +915,7 @@
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2196,7 +2196,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1124" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1124" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="738" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="732" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -4456,8 +4456,8 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>16</v>
+      <c r="D4">
+        <v>2012</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -4478,8 +4478,8 @@
       <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>16</v>
+      <c r="D5">
+        <v>2012</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -4500,8 +4500,8 @@
       <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>16</v>
+      <c r="D6">
+        <v>2012</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -4522,8 +4522,8 @@
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>16</v>
+      <c r="D7">
+        <v>2012</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -4545,8 +4545,8 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>16</v>
+      <c r="D8">
+        <v>2012</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -4565,8 +4565,8 @@
       <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>16</v>
+      <c r="D9">
+        <v>2012</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -4585,8 +4585,8 @@
       <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>16</v>
+      <c r="D10">
+        <v>2012</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -4605,8 +4605,8 @@
       <c r="C11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>16</v>
+      <c r="D11">
+        <v>2012</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -4656,7 +4656,9 @@
     <row r="15" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="16"/>
@@ -4664,7 +4666,9 @@
     <row r="16" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="16"/>
@@ -4672,7 +4676,9 @@
     <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="16"/>
@@ -4680,7 +4686,9 @@
     <row r="18" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="16"/>
@@ -4688,7 +4696,9 @@
     <row r="19" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
       <c r="G19" s="16"/>
@@ -4696,7 +4706,9 @@
     <row r="20" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
       <c r="G20" s="16"/>
@@ -4704,7 +4716,9 @@
     <row r="21" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="D21" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
       <c r="G21" s="16"/>
@@ -4712,7 +4726,9 @@
     <row r="22" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E22" s="6"/>
       <c r="F22" s="7"/>
       <c r="G22" s="16"/>

</xml_diff>

<commit_message>
Replaced DKE with SHR
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RES_DemandFractions.xlsx
+++ b/SuppXLS/Scen_RES_DemandFractions.xlsx
@@ -69,9 +69,6 @@
     <t>Trans - Insert</t>
   </si>
   <si>
-    <t>DKW</t>
-  </si>
-  <si>
     <t>DEM</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>2012-0</t>
+  </si>
+  <si>
+    <t>SHR</t>
   </si>
 </sst>
 </file>
@@ -4403,7 +4403,7 @@
   <dimension ref="A1:Q67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D11"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4440,30 +4440,30 @@
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>2012</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="18">
         <v>0.25</v>
@@ -4473,19 +4473,19 @@
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>2012</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="18">
         <v>0.05</v>
@@ -4495,19 +4495,19 @@
     </row>
     <row r="6" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>2012</v>
+        <v>8</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="18">
         <v>0.25</v>
@@ -4517,19 +4517,19 @@
     </row>
     <row r="7" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>2012</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>14</v>
       </c>
       <c r="G7" s="18">
         <v>0.45</v>
@@ -4540,19 +4540,19 @@
     </row>
     <row r="8" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>2012</v>
+        <v>8</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="18">
         <v>0.27008297187851787</v>
@@ -4560,19 +4560,19 @@
     </row>
     <row r="9" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>2012</v>
+        <v>8</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="18">
         <v>0.21218133862057575</v>
@@ -4580,19 +4580,19 @@
     </row>
     <row r="10" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>2012</v>
+        <v>8</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="18">
         <v>0.21585504882904244</v>
@@ -4600,19 +4600,19 @@
     </row>
     <row r="11" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>2012</v>
+        <v>8</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="18">
         <v>0.30188064067186043</v>
@@ -4656,9 +4656,6 @@
     <row r="15" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="16"/>
@@ -4666,9 +4663,6 @@
     <row r="16" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="16"/>
@@ -4676,9 +4670,6 @@
     <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="16"/>
@@ -4686,9 +4677,6 @@
     <row r="18" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="16"/>
@@ -4696,9 +4684,6 @@
     <row r="19" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
       <c r="G19" s="16"/>
@@ -4706,9 +4691,6 @@
     <row r="20" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
       <c r="G20" s="16"/>
@@ -4716,9 +4698,6 @@
     <row r="21" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
       <c r="G21" s="16"/>
@@ -4726,9 +4705,6 @@
     <row r="22" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E22" s="6"/>
       <c r="F22" s="7"/>
       <c r="G22" s="16"/>

</xml_diff>

<commit_message>
Split RHMDC into TS
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RES_DemandFractions.xlsx
+++ b/SuppXLS/Scen_RES_DemandFractions.xlsx
@@ -90,9 +90,6 @@
     <t>W</t>
   </si>
   <si>
-    <t>RHD, RHM</t>
-  </si>
-  <si>
     <t>RED, REM</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>SHR</t>
+  </si>
+  <si>
+    <t>RHD, RHM, RHMC</t>
   </si>
 </sst>
 </file>
@@ -4403,7 +4403,7 @@
   <dimension ref="A1:Q67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F4" sqref="F4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4413,7 +4413,7 @@
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4446,7 +4446,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4457,13 +4457,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G4" s="18">
         <v>0.25</v>
@@ -4479,13 +4479,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G5" s="18">
         <v>0.05</v>
@@ -4501,13 +4501,13 @@
         <v>8</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G6" s="18">
         <v>0.25</v>
@@ -4523,13 +4523,13 @@
         <v>8</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G7" s="18">
         <v>0.45</v>
@@ -4546,13 +4546,13 @@
         <v>8</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="18">
         <v>0.27008297187851787</v>
@@ -4566,13 +4566,13 @@
         <v>8</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" s="18">
         <v>0.21218133862057575</v>
@@ -4586,13 +4586,13 @@
         <v>8</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="18">
         <v>0.21585504882904244</v>
@@ -4606,13 +4606,13 @@
         <v>8</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="18">
         <v>0.30188064067186043</v>

</xml_diff>